<commit_message>
Added no loops check (V2 commit)
See analysis in showcase_assets > excel file

I also let built binaries (in showcase assets) if anyone finds this and wanna try.
</commit_message>
<xml_diff>
--- a/showcase assets/IQ_circuit_solver_stats.xlsx
+++ b/showcase assets/IQ_circuit_solver_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Projets_persos\Prog\C\IQ_circuit_solver\showcase assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3899ACDE-DB02-4860-A978-C0EFABE2B175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3F5F02-7195-4B45-A4E0-6E74CB1B7228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{22D5D88B-9009-499F-A617-719D769432EB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{22D5D88B-9009-499F-A617-719D769432EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup comments" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Level_num</t>
   </si>
@@ -96,12 +96,30 @@
   <si>
     <t>let's also include Python version here</t>
   </si>
+  <si>
+    <t>v2 : added no loops check</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>green background = gain in performance compared to previous version</t>
+  </si>
+  <si>
+    <t>red background = invalid result</t>
+  </si>
+  <si>
+    <t>todo : maybe a gain table</t>
+  </si>
+  <si>
+    <t>like difference between the number of boards for each levels, where we can see the exact number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +135,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +179,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -312,182 +354,102 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -682,8 +644,155 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>135254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2211705</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E793113-C2EB-46E4-9392-BC53ECAFBD63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="14622779"/>
+          <a:ext cx="4907280" cy="4960621"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>V1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> -&gt; V2 comments </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Supposition : </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Path loops are such a rare case, that I don't feel like it will change much to the number of valid boards found in the general case.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>But this check is still mandatory, as my alogrithm will consider valid a board with a loop, without the check.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Results : </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>See showcase_assets &gt; V1_wrong_solutions.png to see an illustration of why this check is not skippable. V1 even had found wrong solutions, where the loop is in the final board itself ! (The corresponding levels stats were highlighted in red, in this document). It's funny how it's the same 4 pieces block that is involved in that loop.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Overall, it removed a few boards that the algorithm don't have to explore anymore.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Sometimes, the tradeoff of adding this check is worth it in solving time (the drop in number of boards is enough to solve the level, in less time than V1, example : 120)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Sometimes, the number of boards removed is not enough, and the global solving time is increased compared to V1 (example : 117). Because it now has more checks to apply to every single boards.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1003,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA32E1-4AE2-41F3-A97D-46388028FF7D}">
-  <dimension ref="C2:G80"/>
+  <dimension ref="C2:G88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,6 +1123,7 @@
     <col min="3" max="3" width="15.21875" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1023,715 +1133,971 @@
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>49</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="1">
         <v>39</v>
       </c>
+      <c r="F5" s="30">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="24"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="1">
         <v>50</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="1">
         <v>121</v>
       </c>
+      <c r="F6" s="30">
+        <v>121</v>
+      </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="24"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="1">
         <v>51</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="1">
         <v>575</v>
       </c>
+      <c r="F7" s="30">
+        <v>575</v>
+      </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="24"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="1">
         <v>52</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="1">
         <v>45</v>
       </c>
+      <c r="F8" s="30">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="24"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="1">
         <v>53</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="1">
         <v>80</v>
       </c>
+      <c r="F9" s="30">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="24"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="1">
         <v>54</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="1">
         <v>70</v>
       </c>
+      <c r="F10" s="30">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="24"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="1">
         <v>55</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="1">
         <v>87</v>
       </c>
+      <c r="F11" s="30">
+        <v>87</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="24"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="1">
         <v>56</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="1">
         <v>75</v>
       </c>
+      <c r="F12" s="30">
+        <v>75</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="24"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="1">
         <v>57</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="1">
         <v>133</v>
       </c>
+      <c r="F13" s="30">
+        <v>133</v>
+      </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="24"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="1">
         <v>58</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="1">
         <v>801</v>
       </c>
+      <c r="F14" s="30">
+        <v>801</v>
+      </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="24"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="1">
         <v>59</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="1">
         <v>194</v>
       </c>
+      <c r="F15" s="30">
+        <v>194</v>
+      </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="24"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="1">
         <v>60</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="24"/>
+      <c r="F16" s="30">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
       <c r="D17" s="1">
         <v>61</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="24"/>
+      <c r="F17" s="30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
       <c r="D18" s="1">
         <v>62</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="24"/>
+      <c r="F18" s="30">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
       <c r="D19" s="1">
         <v>63</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="24"/>
+      <c r="F19" s="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="17"/>
       <c r="D20" s="1">
         <v>64</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="24"/>
+      <c r="F20" s="30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="17"/>
       <c r="D21" s="1">
         <v>65</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="24"/>
+      <c r="F21" s="30">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="17"/>
       <c r="D22" s="1">
         <v>66</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="1">
         <v>216</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="24"/>
+      <c r="F22" s="30">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="17"/>
       <c r="D23" s="1">
         <v>67</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="24"/>
+      <c r="F23" s="30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="17"/>
       <c r="D24" s="1">
         <v>68</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="24"/>
+      <c r="F24" s="30">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="17"/>
       <c r="D25" s="1">
         <v>69</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="1">
         <v>6689</v>
       </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="24"/>
+      <c r="F25" s="30">
+        <v>6689</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="17"/>
       <c r="D26" s="1">
         <v>70</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="1">
         <v>2555</v>
       </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="24"/>
+      <c r="F26" s="30">
+        <v>2555</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="17"/>
       <c r="D27" s="1">
         <v>71</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="1">
         <v>186</v>
       </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="24"/>
+      <c r="F27" s="30">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="17"/>
       <c r="D28" s="1">
         <v>72</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="24"/>
+      <c r="F28" s="30">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="17"/>
       <c r="D29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="3">
         <f>AVERAGE(E5:E28)</f>
         <v>518.375</v>
       </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="24" t="s">
+      <c r="F29" s="6">
+        <f>AVERAGE(F5:F28)</f>
+        <v>518.375</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="1">
         <v>73</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="1">
         <v>640</v>
       </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="24"/>
+      <c r="F30" s="30">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="17"/>
       <c r="D31" s="1">
         <v>74</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="1">
         <v>184</v>
       </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="24"/>
+      <c r="F31" s="30">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="17"/>
       <c r="D32" s="1">
         <v>75</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="1">
         <v>312</v>
       </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C33" s="24"/>
+      <c r="F32" s="30">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="17"/>
       <c r="D33" s="1">
         <v>76</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="24"/>
+      <c r="F33" s="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="17"/>
       <c r="D34" s="1">
         <v>77</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="1">
         <v>85119</v>
       </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C35" s="24"/>
+      <c r="F34" s="30">
+        <v>85119</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="17"/>
       <c r="D35" s="1">
         <v>78</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="1">
         <v>1301441</v>
       </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C36" s="24"/>
+      <c r="F35" s="36">
+        <v>1301401</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="17"/>
       <c r="D36" s="1">
         <v>79</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="1">
         <v>190</v>
       </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C37" s="24"/>
+      <c r="F36" s="36">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="17"/>
       <c r="D37" s="1">
         <v>80</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C38" s="24"/>
+      <c r="F37" s="30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="17"/>
       <c r="D38" s="1">
         <v>81</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="1">
         <v>54499</v>
       </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C39" s="24"/>
+      <c r="F38" s="36">
+        <v>54493</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="17"/>
       <c r="D39" s="1">
         <v>82</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C40" s="24"/>
+      <c r="F39" s="30">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="17"/>
       <c r="D40" s="1">
         <v>83</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="1">
         <v>2396</v>
       </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C41" s="24"/>
+      <c r="F40" s="30">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="17"/>
       <c r="D41" s="1">
         <v>84</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C42" s="24"/>
+      <c r="F41" s="30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="17"/>
       <c r="D42" s="1">
         <v>85</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="1">
         <v>5859</v>
       </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C43" s="24"/>
+      <c r="F42" s="30">
+        <v>5859</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="17"/>
       <c r="D43" s="1">
         <v>86</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="1">
         <v>1391</v>
       </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C44" s="24"/>
+      <c r="F43" s="30">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="17"/>
       <c r="D44" s="1">
         <v>87</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="1">
         <v>17023</v>
       </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C45" s="24"/>
+      <c r="F44" s="36">
+        <v>16999</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="17"/>
       <c r="D45" s="1">
         <v>88</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="1">
         <v>1037611</v>
       </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C46" s="24"/>
+      <c r="F45" s="36">
+        <v>958157</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="17"/>
       <c r="D46" s="1">
         <v>89</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="1">
         <v>1132903</v>
       </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C47" s="24"/>
+      <c r="F46" s="36">
+        <v>1132823</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="17"/>
       <c r="D47" s="1">
         <v>90</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="1">
         <v>131525</v>
       </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C48" s="24"/>
+      <c r="F47" s="36">
+        <v>131523</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="17"/>
       <c r="D48" s="1">
         <v>91</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="1">
         <v>47722</v>
       </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C49" s="24"/>
+      <c r="F48" s="30">
+        <v>47722</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="17"/>
       <c r="D49" s="1">
         <v>92</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="26">
         <v>21702</v>
       </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C50" s="24"/>
+      <c r="F49" s="31">
+        <v>118082</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="17"/>
       <c r="D50" s="1">
         <v>93</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="1">
         <v>3742</v>
       </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C51" s="24"/>
+      <c r="F50" s="36">
+        <v>3729</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="17"/>
       <c r="D51" s="1">
         <v>94</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="1">
         <v>31438</v>
       </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C52" s="24"/>
+      <c r="F51" s="36">
+        <v>30968</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="17"/>
       <c r="D52" s="1">
         <v>95</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="1">
         <v>4239</v>
       </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C53" s="24"/>
+      <c r="F52" s="30">
+        <v>4239</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="17"/>
       <c r="D53" s="1">
         <v>96</v>
       </c>
-      <c r="E53" s="10">
+      <c r="E53" s="1">
         <v>17317</v>
       </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C54" s="24"/>
+      <c r="F53" s="36">
+        <v>17136</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="17"/>
       <c r="D54" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="3">
         <f>AVERAGE(E30:E53)</f>
         <v>162396.5</v>
       </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C55" s="24" t="s">
+      <c r="F54" s="6">
+        <f>AVERAGE(F30:F53)</f>
+        <v>163067.70833333334</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C55" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D55" s="1">
         <v>97</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55" s="1">
         <v>4191</v>
       </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C56" s="24"/>
+      <c r="F55" s="36">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="17"/>
       <c r="D56" s="1">
         <v>98</v>
       </c>
-      <c r="E56" s="10">
+      <c r="E56" s="26">
         <v>33908</v>
       </c>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C57" s="24"/>
+      <c r="F56" s="31">
+        <v>203882</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C57" s="17"/>
       <c r="D57" s="1">
         <v>99</v>
       </c>
-      <c r="E57" s="10">
+      <c r="E57" s="1">
         <v>489</v>
       </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C58" s="24"/>
+      <c r="F57" s="36">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="17"/>
       <c r="D58" s="1">
         <v>100</v>
       </c>
-      <c r="E58" s="10">
+      <c r="E58" s="1">
         <v>342937</v>
       </c>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C59" s="24"/>
+      <c r="F58" s="36">
+        <v>340536</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C59" s="17"/>
       <c r="D59" s="1">
         <v>101</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59" s="1">
         <v>10912</v>
       </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C60" s="24"/>
+      <c r="F59" s="36">
+        <v>10842</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="17"/>
       <c r="D60" s="1">
         <v>102</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="1">
         <v>1559</v>
       </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C61" s="24"/>
+      <c r="F60" s="36">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C61" s="17"/>
       <c r="D61" s="1">
         <v>103</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E61" s="1">
         <v>17176</v>
       </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C62" s="24"/>
+      <c r="F61" s="30">
+        <v>17176</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="17"/>
       <c r="D62" s="1">
         <v>104</v>
       </c>
-      <c r="E62" s="10">
+      <c r="E62" s="1">
         <v>2968</v>
       </c>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C63" s="24"/>
+      <c r="F62" s="30">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C63" s="17"/>
       <c r="D63" s="1">
         <v>105</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63" s="1">
         <v>46496</v>
       </c>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C64" s="24"/>
+      <c r="F63" s="36">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C64" s="17"/>
       <c r="D64" s="1">
         <v>106</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="1">
         <v>11120306</v>
       </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C65" s="24"/>
+      <c r="F64" s="36">
+        <v>10929800</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C65" s="17"/>
       <c r="D65" s="1">
         <v>107</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="1">
         <v>1029</v>
       </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="24"/>
+      <c r="F65" s="30">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C66" s="17"/>
       <c r="D66" s="1">
         <v>108</v>
       </c>
-      <c r="E66" s="10">
+      <c r="E66" s="1">
         <v>117348</v>
       </c>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C67" s="24"/>
+      <c r="F66" s="36">
+        <v>114456</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C67" s="17"/>
       <c r="D67" s="1">
         <v>109</v>
       </c>
-      <c r="E67" s="10">
+      <c r="E67" s="1">
         <v>238800</v>
       </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C68" s="24"/>
+      <c r="F67" s="36">
+        <v>233931</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C68" s="17"/>
       <c r="D68" s="1">
         <v>110</v>
       </c>
-      <c r="E68" s="10">
+      <c r="E68" s="1">
         <v>134882</v>
       </c>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C69" s="24"/>
+      <c r="F68" s="36">
+        <v>134500</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="17"/>
       <c r="D69" s="1">
         <v>111</v>
       </c>
-      <c r="E69" s="10">
+      <c r="E69" s="1">
         <v>12276</v>
       </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C70" s="24"/>
+      <c r="F69" s="30">
+        <v>12276</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="17"/>
       <c r="D70" s="1">
         <v>112</v>
       </c>
-      <c r="E70" s="10">
+      <c r="E70" s="1">
         <v>232789</v>
       </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C71" s="24"/>
+      <c r="F70" s="36">
+        <v>229232</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="17"/>
       <c r="D71" s="1">
         <v>113</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E71" s="1">
         <v>472494</v>
       </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C72" s="24"/>
+      <c r="F71" s="36">
+        <v>464960</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="17"/>
       <c r="D72" s="1">
         <v>114</v>
       </c>
-      <c r="E72" s="10">
+      <c r="E72" s="1">
         <v>250974</v>
       </c>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C73" s="24"/>
+      <c r="F72" s="36">
+        <v>248465</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="17"/>
       <c r="D73" s="1">
         <v>115</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E73" s="1">
         <v>7438336</v>
       </c>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C74" s="24"/>
+      <c r="F73" s="36">
+        <v>7391077</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="17"/>
       <c r="D74" s="1">
         <v>116</v>
       </c>
-      <c r="E74" s="10">
+      <c r="E74" s="1">
         <v>1204664</v>
       </c>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C75" s="24"/>
+      <c r="F74" s="36">
+        <v>1204501</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C75" s="17"/>
       <c r="D75" s="1">
         <v>117</v>
       </c>
-      <c r="E75" s="10">
+      <c r="E75" s="1">
         <v>22543339</v>
       </c>
-    </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C76" s="24"/>
+      <c r="F75" s="36">
+        <v>22394763</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C76" s="17"/>
       <c r="D76" s="1">
         <v>118</v>
       </c>
-      <c r="E76" s="10">
+      <c r="E76" s="1">
         <v>21709270</v>
       </c>
-    </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C77" s="24"/>
+      <c r="F76" s="36">
+        <v>21365971</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C77" s="17"/>
       <c r="D77" s="1">
         <v>119</v>
       </c>
-      <c r="E77" s="10">
+      <c r="E77" s="26">
         <v>9633721</v>
       </c>
-    </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C78" s="24"/>
+      <c r="F77" s="31">
+        <v>34341801</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C78" s="17"/>
       <c r="D78" s="1">
         <v>120</v>
       </c>
-      <c r="E78" s="10">
+      <c r="E78" s="1">
         <v>23211009</v>
       </c>
-    </row>
-    <row r="79" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C79" s="26"/>
-      <c r="D79" s="4" t="s">
+      <c r="F78" s="36">
+        <v>22868995</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C79" s="17"/>
+      <c r="D79" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E79" s="27">
+      <c r="E79" s="3">
         <f>AVERAGE(E55:E78)</f>
         <v>4115911.375</v>
       </c>
-    </row>
-    <row r="80" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C80" s="19" t="s">
+      <c r="F79" s="6">
+        <f>AVERAGE(F55:F78)</f>
+        <v>5106807.583333333</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C80" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21">
+      <c r="D80" s="33"/>
+      <c r="E80" s="34">
         <f>(AVERAGE(E29,E54,E79))</f>
         <v>1426275.4166666667</v>
+      </c>
+      <c r="F80" s="35">
+        <f>(AVERAGE(F29,F54,F79))</f>
+        <v>1756797.8888888888</v>
+      </c>
+    </row>
+    <row r="84" spans="5:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E84" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="5:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E85" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E87" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="5:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E88" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1740,8 +2106,9 @@
     <mergeCell ref="C30:C54"/>
     <mergeCell ref="C55:C79"/>
     <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C3:F3"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C3:E3" location="'IQ circuit solver C version'!A1" display="C version" xr:uid="{C1B8BCA1-31BC-4420-BEE0-9684C3557F53}"/>
   </hyperlinks>
@@ -1751,1154 +2118,1834 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE79279-43FE-4514-886C-88FC286043C2}">
-  <dimension ref="C2:G81"/>
+  <dimension ref="C2:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="6" max="6" width="34.88671875" customWidth="1"/>
-    <col min="7" max="7" width="32.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="5" t="s">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="H3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="7">
         <v>49</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="7">
         <v>39</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="7">
         <v>0</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="7">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
-      <c r="D5" s="1">
+      <c r="H4" s="7">
+        <v>39</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="24"/>
+      <c r="D5" s="7">
         <v>50</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="7">
         <v>121</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="7">
         <v>0</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="7">
         <v>201</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="1">
+      <c r="H5" s="7">
+        <v>121</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="24"/>
+      <c r="D6" s="7">
         <v>51</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="7">
         <v>575</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="7">
         <v>2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="7">
         <v>653</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
-      <c r="D7" s="1">
+      <c r="H6" s="7">
+        <v>575</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="24"/>
+      <c r="D7" s="7">
         <v>52</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="7">
         <v>45</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="7">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="7">
         <v>147</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="1">
+      <c r="H7" s="7">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="24"/>
+      <c r="D8" s="7">
         <v>53</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="7">
         <v>80</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="7">
         <v>123</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
-      <c r="D9" s="1">
+      <c r="H8" s="7">
+        <v>80</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="24"/>
+      <c r="D9" s="7">
         <v>54</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="7">
         <v>70</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="7">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
-      <c r="D10" s="1">
+      <c r="H9" s="7">
+        <v>70</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="24"/>
+      <c r="D10" s="7">
         <v>55</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="7">
         <v>87</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="7">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="7">
         <v>174</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
-      <c r="D11" s="1">
+      <c r="H10" s="7">
+        <v>87</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="24"/>
+      <c r="D11" s="7">
         <v>56</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="7">
         <v>75</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="7">
         <v>155</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="1">
+      <c r="H11" s="7">
+        <v>75</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="24"/>
+      <c r="D12" s="7">
         <v>57</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="7">
         <v>133</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="7">
         <v>1</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="7">
         <v>216</v>
       </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
-      <c r="D13" s="1">
+      <c r="H12" s="7">
+        <v>133</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="24"/>
+      <c r="D13" s="7">
         <v>58</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="7">
         <v>801</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="7">
         <v>3</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="7">
         <v>849</v>
       </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="1">
+      <c r="H13" s="7">
+        <v>801</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="7">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="24"/>
+      <c r="D14" s="7">
         <v>59</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="7">
         <v>194</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="7">
         <v>1</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="7">
         <v>273</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="1">
+      <c r="H14" s="7">
+        <v>194</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="24"/>
+      <c r="D15" s="7">
         <v>60</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="7">
         <v>70</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="7">
         <v>0</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="7">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
-      <c r="D16" s="1">
+      <c r="H15" s="7">
+        <v>70</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="24"/>
+      <c r="D16" s="7">
         <v>61</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="7">
         <v>150</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="7">
         <v>240</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
-      <c r="D17" s="1">
+      <c r="H16" s="7">
+        <v>150</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="24"/>
+      <c r="D17" s="7">
         <v>62</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="7">
         <v>78</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="7">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="1">
+      <c r="H17" s="7">
+        <v>78</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C18" s="24"/>
+      <c r="D18" s="7">
         <v>63</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="7">
         <v>11</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="7">
         <v>0</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="7">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="6"/>
-      <c r="D19" s="1">
+      <c r="H18" s="7">
+        <v>11</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C19" s="24"/>
+      <c r="D19" s="7">
         <v>64</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="7">
         <v>79</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="7">
         <v>1</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="7">
         <v>164</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="1">
+      <c r="H19" s="7">
+        <v>79</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="24"/>
+      <c r="D20" s="7">
         <v>65</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="7">
         <v>74</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="7">
         <v>0</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="7">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="6"/>
-      <c r="D21" s="1">
+      <c r="H20" s="7">
+        <v>74</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C21" s="24"/>
+      <c r="D21" s="7">
         <v>66</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="7">
         <v>216</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="7">
         <v>1</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="7">
         <v>306</v>
       </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C22" s="6"/>
-      <c r="D22" s="1">
+      <c r="H21" s="7">
+        <v>216</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="7">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="24"/>
+      <c r="D22" s="7">
         <v>67</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="7">
         <v>22</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="7">
         <v>0</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C23" s="6"/>
-      <c r="D23" s="1">
+      <c r="H22" s="7">
+        <v>22</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C23" s="24"/>
+      <c r="D23" s="7">
         <v>68</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="7">
         <v>44</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="7">
         <v>0</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="7">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="6"/>
-      <c r="D24" s="1">
+      <c r="H23" s="7">
+        <v>44</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C24" s="24"/>
+      <c r="D24" s="7">
         <v>69</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="7">
         <v>6689</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="7">
         <v>31</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="7">
         <v>6335</v>
       </c>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="6"/>
-      <c r="D25" s="1">
+      <c r="H24" s="7">
+        <v>6689</v>
+      </c>
+      <c r="I24" s="1">
+        <v>24</v>
+      </c>
+      <c r="J24" s="7">
+        <v>6512</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C25" s="24"/>
+      <c r="D25" s="7">
         <v>70</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="7">
         <v>2555</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="7">
         <v>11</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="7">
         <v>2481</v>
       </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C26" s="6"/>
-      <c r="D26" s="1">
+      <c r="H25" s="7">
+        <v>2555</v>
+      </c>
+      <c r="I25" s="1">
+        <v>9</v>
+      </c>
+      <c r="J25" s="7">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="24"/>
+      <c r="D26" s="7">
         <v>71</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="7">
         <v>186</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="7">
         <v>1</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="7">
         <v>275</v>
       </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C27" s="6"/>
-      <c r="D27" s="1">
+      <c r="H26" s="7">
+        <v>186</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C27" s="24"/>
+      <c r="D27" s="7">
         <v>72</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="7">
         <v>47</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="7">
         <v>0</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="7">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
-      <c r="D28" s="3" t="s">
+      <c r="H27" s="7">
+        <v>47</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C28" s="24"/>
+      <c r="D28" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="10">
         <f>AVERAGE(E4:E27)</f>
         <v>518.375</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="10">
         <f>AVERAGE(F4:F27)</f>
         <v>2.4583333333333335</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="10">
         <f>AVERAGE(G4:G27)</f>
         <v>545</v>
       </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C29" s="6" t="s">
+      <c r="H28" s="10">
+        <f t="shared" ref="H28:J28" si="0">AVERAGE(H4:H27)</f>
+        <v>518.375</v>
+      </c>
+      <c r="I28" s="10">
+        <f t="shared" si="0"/>
+        <v>1.875</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="0"/>
+        <v>547.08333333333337</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C29" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="7">
         <v>73</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="7">
         <v>640</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="7">
         <v>2</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="7">
         <v>704</v>
       </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C30" s="6"/>
-      <c r="D30" s="1">
+      <c r="H29" s="7">
+        <v>640</v>
+      </c>
+      <c r="I29" s="7">
+        <v>2</v>
+      </c>
+      <c r="J29" s="1">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C30" s="24"/>
+      <c r="D30" s="7">
         <v>74</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="7">
         <v>184</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="7">
         <v>1</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="7">
         <v>255</v>
       </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C31" s="6"/>
-      <c r="D31" s="1">
+      <c r="H30" s="7">
+        <v>184</v>
+      </c>
+      <c r="I30" s="7">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C31" s="24"/>
+      <c r="D31" s="7">
         <v>75</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="7">
         <v>312</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="7">
         <v>1</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="7">
         <v>386</v>
       </c>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C32" s="6"/>
-      <c r="D32" s="1">
+      <c r="H31" s="7">
+        <v>312</v>
+      </c>
+      <c r="I31" s="7">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C32" s="24"/>
+      <c r="D32" s="7">
         <v>76</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="7">
         <v>18</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="7">
         <v>0</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C33" s="6"/>
-      <c r="D33" s="1">
+      <c r="H32" s="7">
+        <v>18</v>
+      </c>
+      <c r="I32" s="7">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C33" s="24"/>
+      <c r="D33" s="7">
         <v>77</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="7">
         <v>85119</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="7">
         <v>224</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="7">
         <v>79368</v>
       </c>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C34" s="6"/>
-      <c r="D34" s="1">
+      <c r="H33" s="7">
+        <v>85119</v>
+      </c>
+      <c r="I33" s="7">
+        <v>237</v>
+      </c>
+      <c r="J33" s="1">
+        <v>79525</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C34" s="24"/>
+      <c r="D34" s="7">
         <v>78</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="7">
         <v>1301441</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="7">
         <v>4000</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="7">
         <v>1276897</v>
       </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C35" s="6"/>
-      <c r="D35" s="1">
+      <c r="H34" s="7">
+        <v>1301401</v>
+      </c>
+      <c r="I34" s="7">
+        <v>4138</v>
+      </c>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="24"/>
+      <c r="D35" s="7">
         <v>79</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="7">
         <v>190</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="7">
         <v>1</v>
       </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C36" s="6"/>
-      <c r="D36" s="1">
+      <c r="G35" s="7"/>
+      <c r="H35" s="7">
+        <v>189</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C36" s="24"/>
+      <c r="D36" s="7">
         <v>80</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="7">
         <v>38</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="7">
         <v>0</v>
       </c>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C37" s="6"/>
-      <c r="D37" s="1">
+      <c r="G36" s="7"/>
+      <c r="H36" s="7">
+        <v>38</v>
+      </c>
+      <c r="I36" s="7">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C37" s="24"/>
+      <c r="D37" s="7">
         <v>81</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="7">
         <v>54499</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="7">
         <v>223</v>
       </c>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C38" s="6"/>
-      <c r="D38" s="1">
+      <c r="G37" s="7"/>
+      <c r="H37" s="7">
+        <v>54493</v>
+      </c>
+      <c r="I37" s="7">
+        <v>213</v>
+      </c>
+      <c r="J37" s="1">
+        <v>51398</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C38" s="24"/>
+      <c r="D38" s="7">
         <v>82</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="7">
         <v>176</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="7">
         <v>1</v>
       </c>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C39" s="6"/>
-      <c r="D39" s="1">
+      <c r="G38" s="7"/>
+      <c r="H38" s="7">
+        <v>176</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C39" s="24"/>
+      <c r="D39" s="7">
         <v>83</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="7">
         <v>2396</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="7">
         <v>9</v>
       </c>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C40" s="6"/>
-      <c r="D40" s="1">
+      <c r="G39" s="7"/>
+      <c r="H39" s="7">
+        <v>2396</v>
+      </c>
+      <c r="I39" s="7">
+        <v>9</v>
+      </c>
+      <c r="J39" s="1">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C40" s="24"/>
+      <c r="D40" s="7">
         <v>84</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="7">
         <v>31</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="7">
         <v>0</v>
       </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C41" s="6"/>
-      <c r="D41" s="1">
+      <c r="G40" s="7"/>
+      <c r="H40" s="7">
+        <v>31</v>
+      </c>
+      <c r="I40" s="7">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C41" s="24"/>
+      <c r="D41" s="7">
         <v>85</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="7">
         <v>5859</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="7">
         <v>19</v>
       </c>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C42" s="6"/>
-      <c r="D42" s="1">
+      <c r="G41" s="7"/>
+      <c r="H41" s="7">
+        <v>5859</v>
+      </c>
+      <c r="I41" s="7">
+        <v>20</v>
+      </c>
+      <c r="J41" s="1">
+        <v>5637</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C42" s="24"/>
+      <c r="D42" s="7">
         <v>86</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="7">
         <v>1391</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="7">
         <v>5</v>
       </c>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C43" s="6"/>
-      <c r="D43" s="1">
+      <c r="G42" s="7"/>
+      <c r="H42" s="7">
+        <v>1391</v>
+      </c>
+      <c r="I42" s="7">
+        <v>5</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C43" s="24"/>
+      <c r="D43" s="7">
         <v>87</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="7">
         <v>17023</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="7">
         <v>86</v>
       </c>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C44" s="6"/>
-      <c r="D44" s="1">
+      <c r="G43" s="7"/>
+      <c r="H43" s="7">
+        <v>16999</v>
+      </c>
+      <c r="I43" s="7">
+        <v>66</v>
+      </c>
+      <c r="J43" s="1">
+        <v>16747</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C44" s="24"/>
+      <c r="D44" s="7">
         <v>88</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="7">
         <v>1037611</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="7">
         <v>3728</v>
       </c>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C45" s="6"/>
-      <c r="D45" s="1">
+      <c r="G44" s="7"/>
+      <c r="H44" s="7">
+        <v>958157</v>
+      </c>
+      <c r="I44" s="7">
+        <v>3479</v>
+      </c>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C45" s="24"/>
+      <c r="D45" s="7">
         <v>89</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="7">
         <v>1132903</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="7">
         <v>4067</v>
       </c>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C46" s="6"/>
-      <c r="D46" s="1">
+      <c r="G45" s="7"/>
+      <c r="H45" s="7">
+        <v>1132823</v>
+      </c>
+      <c r="I45" s="7">
+        <v>3229</v>
+      </c>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C46" s="24"/>
+      <c r="D46" s="7">
         <v>90</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="7">
         <v>131525</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="7">
         <v>491</v>
       </c>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C47" s="6"/>
-      <c r="D47" s="1">
+      <c r="G46" s="7"/>
+      <c r="H46" s="7">
+        <v>131523</v>
+      </c>
+      <c r="I46" s="7">
+        <v>435</v>
+      </c>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C47" s="24"/>
+      <c r="D47" s="7">
         <v>91</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="7">
         <v>47722</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="7">
         <v>204</v>
       </c>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C48" s="6"/>
-      <c r="D48" s="1">
+      <c r="G47" s="7"/>
+      <c r="H47" s="7">
+        <v>47722</v>
+      </c>
+      <c r="I47" s="7">
+        <v>157</v>
+      </c>
+      <c r="J47" s="7">
+        <v>47111</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C48" s="24"/>
+      <c r="D48" s="7">
         <v>92</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="16">
         <v>21702</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="16">
         <v>72</v>
       </c>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C49" s="6"/>
-      <c r="D49" s="1">
+      <c r="G48" s="16"/>
+      <c r="H48" s="25">
+        <v>118082</v>
+      </c>
+      <c r="I48" s="7">
+        <v>298</v>
+      </c>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C49" s="24"/>
+      <c r="D49" s="7">
         <v>93</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="7">
         <v>3742</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="7">
         <v>16</v>
       </c>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C50" s="6"/>
-      <c r="D50" s="1">
+      <c r="G49" s="7"/>
+      <c r="H49" s="7">
+        <v>3729</v>
+      </c>
+      <c r="I49" s="7">
+        <v>13</v>
+      </c>
+      <c r="J49" s="1">
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C50" s="24"/>
+      <c r="D50" s="7">
         <v>94</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="7">
         <v>31438</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="7">
         <v>97</v>
       </c>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C51" s="6"/>
-      <c r="D51" s="1">
+      <c r="G50" s="7"/>
+      <c r="H50" s="7">
+        <v>30968</v>
+      </c>
+      <c r="I50" s="7">
+        <v>100</v>
+      </c>
+      <c r="J50" s="1">
+        <v>30459</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C51" s="24"/>
+      <c r="D51" s="7">
         <v>95</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="7">
         <v>4239</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="7">
         <v>14</v>
       </c>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C52" s="6"/>
-      <c r="D52" s="1">
+      <c r="G51" s="7"/>
+      <c r="H51" s="7">
+        <v>4239</v>
+      </c>
+      <c r="I51" s="7">
+        <v>14</v>
+      </c>
+      <c r="J51" s="1">
+        <v>4493</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C52" s="24"/>
+      <c r="D52" s="7">
         <v>96</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="7">
         <v>17317</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="7">
         <v>82</v>
       </c>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C53" s="6"/>
-      <c r="D53" s="3" t="s">
+      <c r="G52" s="7"/>
+      <c r="H52" s="7">
+        <v>17136</v>
+      </c>
+      <c r="I52" s="7">
+        <v>61</v>
+      </c>
+      <c r="J52" s="1">
+        <v>16889</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C53" s="24"/>
+      <c r="D53" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="10">
         <f>AVERAGE(E29:E52)</f>
         <v>162396.5</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="10">
         <f>AVERAGE(F29:F52)</f>
         <v>555.95833333333337</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="10">
         <f>AVERAGE(G29:G52)</f>
         <v>226271.66666666666</v>
       </c>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C54" s="6" t="s">
+      <c r="H53" s="10">
+        <f t="shared" ref="H53:I53" si="1">AVERAGE(H29:H52)</f>
+        <v>163067.70833333334</v>
+      </c>
+      <c r="I53" s="10">
+        <f t="shared" si="1"/>
+        <v>520</v>
+      </c>
+      <c r="J53" s="10">
+        <f>AVERAGE(J29:J52)</f>
+        <v>13797.894736842105</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C54" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="7">
         <v>97</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="7">
         <v>4191</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F54" s="7">
         <v>15</v>
       </c>
-      <c r="G54" s="1">
+      <c r="G54" s="7">
         <v>3992</v>
       </c>
-    </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C55" s="6"/>
-      <c r="D55" s="1">
+      <c r="H54" s="7">
+        <v>4190</v>
+      </c>
+      <c r="I54" s="7">
+        <v>17</v>
+      </c>
+      <c r="J54" s="7">
+        <v>4222</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C55" s="24"/>
+      <c r="D55" s="7">
         <v>98</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="16">
         <v>33908</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="16">
         <v>150</v>
       </c>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C56" s="6"/>
-      <c r="D56" s="1">
+      <c r="G55" s="16"/>
+      <c r="H55" s="25">
+        <v>203882</v>
+      </c>
+      <c r="I55" s="7">
+        <v>732</v>
+      </c>
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C56" s="24"/>
+      <c r="D56" s="7">
         <v>99</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="7">
         <v>489</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56" s="7">
         <v>3</v>
       </c>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C57" s="6"/>
-      <c r="D57" s="1">
+      <c r="G56" s="7"/>
+      <c r="H56" s="7">
+        <v>487</v>
+      </c>
+      <c r="I56" s="7">
+        <v>2</v>
+      </c>
+      <c r="J56" s="7">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C57" s="24"/>
+      <c r="D57" s="7">
         <v>100</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="7">
         <v>342937</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57" s="7">
         <v>1169</v>
       </c>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C58" s="6"/>
-      <c r="D58" s="1">
+      <c r="G57" s="7"/>
+      <c r="H57" s="7">
+        <v>340536</v>
+      </c>
+      <c r="I57" s="7">
+        <v>1163</v>
+      </c>
+      <c r="J57" s="7"/>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C58" s="24"/>
+      <c r="D58" s="7">
         <v>101</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="7">
         <v>10912</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F58" s="7">
         <v>52</v>
       </c>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C59" s="6"/>
-      <c r="D59" s="1">
+      <c r="G58" s="7"/>
+      <c r="H58" s="7">
+        <v>10842</v>
+      </c>
+      <c r="I58" s="7">
+        <v>42</v>
+      </c>
+      <c r="J58" s="1">
+        <v>11117</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C59" s="24"/>
+      <c r="D59" s="7">
         <v>102</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="7">
         <v>1559</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="7">
         <v>5</v>
       </c>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C60" s="6"/>
-      <c r="D60" s="1">
+      <c r="G59" s="7"/>
+      <c r="H59" s="7">
+        <v>1557</v>
+      </c>
+      <c r="I59" s="7">
+        <v>6</v>
+      </c>
+      <c r="J59" s="1">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C60" s="24"/>
+      <c r="D60" s="7">
         <v>103</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="7">
         <v>17176</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60" s="7">
         <v>70</v>
       </c>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C61" s="6"/>
-      <c r="D61" s="1">
+      <c r="G60" s="7"/>
+      <c r="H60" s="7">
+        <v>17176</v>
+      </c>
+      <c r="I60" s="7">
+        <v>77</v>
+      </c>
+      <c r="J60" s="1">
+        <v>17252</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C61" s="24"/>
+      <c r="D61" s="7">
         <v>104</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="7">
         <v>2968</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="7">
         <v>13</v>
       </c>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C62" s="6"/>
-      <c r="D62" s="1">
+      <c r="G61" s="7"/>
+      <c r="H61" s="7">
+        <v>2968</v>
+      </c>
+      <c r="I61" s="7">
+        <v>12</v>
+      </c>
+      <c r="J61" s="1">
+        <v>3052</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C62" s="24"/>
+      <c r="D62" s="7">
         <v>105</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="7">
         <v>46496</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="7">
         <v>208</v>
       </c>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C63" s="6"/>
-      <c r="D63" s="1">
+      <c r="G62" s="7"/>
+      <c r="H62" s="7">
+        <v>45987</v>
+      </c>
+      <c r="I62" s="7">
+        <v>177</v>
+      </c>
+      <c r="J62" s="1">
+        <v>46172</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C63" s="24"/>
+      <c r="D63" s="7">
         <v>106</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="7">
         <v>11120306</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="7">
         <v>39173</v>
       </c>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C64" s="6"/>
-      <c r="D64" s="1">
+      <c r="G63" s="7"/>
+      <c r="H63" s="7">
+        <v>10929800</v>
+      </c>
+      <c r="I63" s="7">
+        <v>34609</v>
+      </c>
+      <c r="J63" s="7"/>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C64" s="24"/>
+      <c r="D64" s="7">
         <v>107</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="7">
         <v>1029</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64" s="7">
         <v>5</v>
       </c>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C65" s="6"/>
-      <c r="D65" s="1">
+      <c r="G64" s="7"/>
+      <c r="H64" s="7">
+        <v>1029</v>
+      </c>
+      <c r="I64" s="7">
+        <v>4</v>
+      </c>
+      <c r="J64" s="7">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C65" s="24"/>
+      <c r="D65" s="7">
         <v>108</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="7">
         <v>117348</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="7">
         <v>309</v>
       </c>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C66" s="6"/>
-      <c r="D66" s="1">
+      <c r="G65" s="7"/>
+      <c r="H65" s="7">
+        <v>114456</v>
+      </c>
+      <c r="I65" s="7">
+        <v>321</v>
+      </c>
+      <c r="J65" s="7"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C66" s="24"/>
+      <c r="D66" s="7">
         <v>109</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="7">
         <v>238800</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="7">
         <v>936</v>
       </c>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C67" s="6"/>
-      <c r="D67" s="1">
+      <c r="G66" s="7"/>
+      <c r="H66" s="7">
+        <v>233931</v>
+      </c>
+      <c r="I66" s="7">
+        <v>910</v>
+      </c>
+      <c r="J66" s="7"/>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C67" s="24"/>
+      <c r="D67" s="7">
         <v>110</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="7">
         <v>134882</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67" s="7">
         <v>434</v>
       </c>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C68" s="6"/>
-      <c r="D68" s="1">
+      <c r="G67" s="7"/>
+      <c r="H67" s="7">
+        <v>134500</v>
+      </c>
+      <c r="I67" s="7">
+        <v>429</v>
+      </c>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C68" s="24"/>
+      <c r="D68" s="7">
         <v>111</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="7">
         <v>12276</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68" s="7">
         <v>43</v>
       </c>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C69" s="6"/>
-      <c r="D69" s="1">
+      <c r="G68" s="7"/>
+      <c r="H68" s="7">
+        <v>12276</v>
+      </c>
+      <c r="I68" s="7">
+        <v>39</v>
+      </c>
+      <c r="J68" s="7">
+        <v>12576</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C69" s="24"/>
+      <c r="D69" s="7">
         <v>112</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="7">
         <v>232789</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F69" s="7">
         <v>882</v>
       </c>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C70" s="6"/>
-      <c r="D70" s="1">
+      <c r="G69" s="7"/>
+      <c r="H69" s="7">
+        <v>229232</v>
+      </c>
+      <c r="I69" s="7">
+        <v>737</v>
+      </c>
+      <c r="J69" s="7"/>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C70" s="24"/>
+      <c r="D70" s="7">
         <v>113</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="7">
         <v>472494</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70" s="7">
         <v>1683</v>
       </c>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C71" s="6"/>
-      <c r="D71" s="1">
+      <c r="G70" s="7"/>
+      <c r="H70" s="7">
+        <v>464960</v>
+      </c>
+      <c r="I70" s="7">
+        <v>1475</v>
+      </c>
+      <c r="J70" s="7"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C71" s="24"/>
+      <c r="D71" s="7">
         <v>114</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="7">
         <v>250974</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F71" s="7">
         <v>835</v>
       </c>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C72" s="6"/>
-      <c r="D72" s="1">
+      <c r="G71" s="7"/>
+      <c r="H71" s="7">
+        <v>248465</v>
+      </c>
+      <c r="I71" s="7">
+        <v>722</v>
+      </c>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C72" s="24"/>
+      <c r="D72" s="7">
         <v>115</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="7">
         <v>7438336</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72" s="7">
         <v>28190</v>
       </c>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C73" s="6"/>
-      <c r="D73" s="1">
+      <c r="G72" s="7"/>
+      <c r="H72" s="7">
+        <v>7391077</v>
+      </c>
+      <c r="I72" s="7">
+        <v>24232</v>
+      </c>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C73" s="24"/>
+      <c r="D73" s="7">
         <v>116</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="7">
         <v>1204664</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73" s="7">
         <v>4211</v>
       </c>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C74" s="6"/>
-      <c r="D74" s="1">
+      <c r="G73" s="7"/>
+      <c r="H73" s="7">
+        <v>1204501</v>
+      </c>
+      <c r="I73" s="7">
+        <v>4150</v>
+      </c>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C74" s="24"/>
+      <c r="D74" s="7">
         <v>117</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="7">
         <v>22543339</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74" s="7">
         <v>72841</v>
       </c>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C75" s="6"/>
-      <c r="D75" s="1">
+      <c r="G74" s="7"/>
+      <c r="H74" s="7">
+        <v>22394763</v>
+      </c>
+      <c r="I74" s="7">
+        <v>74225</v>
+      </c>
+      <c r="J74" s="7"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C75" s="24"/>
+      <c r="D75" s="7">
         <v>118</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="7">
         <v>21709270</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F75" s="7">
         <v>76869</v>
       </c>
-      <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C76" s="6"/>
-      <c r="D76" s="1">
+      <c r="G75" s="7"/>
+      <c r="H75" s="7">
+        <v>21365971</v>
+      </c>
+      <c r="I75" s="7">
+        <v>72591</v>
+      </c>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C76" s="24"/>
+      <c r="D76" s="7">
         <v>119</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="16">
         <v>9633721</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F76" s="16">
         <v>30763</v>
       </c>
-      <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C77" s="6"/>
-      <c r="D77" s="1">
+      <c r="G76" s="16"/>
+      <c r="H76" s="25">
+        <v>34341801</v>
+      </c>
+      <c r="I76" s="7">
+        <v>101947</v>
+      </c>
+      <c r="J76" s="7"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C77" s="24"/>
+      <c r="D77" s="7">
         <v>120</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="7">
         <v>23211009</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F77" s="7">
         <v>73824</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="G77" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="78" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C78" s="7"/>
-      <c r="D78" s="4" t="s">
+      <c r="H77" s="7">
+        <v>22868995</v>
+      </c>
+      <c r="I77" s="7">
+        <v>69157</v>
+      </c>
+      <c r="J77" s="7"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C78" s="24"/>
+      <c r="D78" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78" s="10">
         <f>AVERAGE(E54:E77)</f>
         <v>4115911.375</v>
       </c>
-      <c r="F78" s="4">
+      <c r="F78" s="10">
         <f xml:space="preserve"> AVERAGE(F54:F77)</f>
         <v>13861.791666666666</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G78" s="10">
         <f xml:space="preserve"> AVERAGE(G54:G77)</f>
         <v>3992</v>
       </c>
-    </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C79" s="15" t="s">
+      <c r="H78" s="10">
+        <f t="shared" ref="H78:J78" si="2" xml:space="preserve"> AVERAGE(H54:H77)</f>
+        <v>5106807.583333333</v>
+      </c>
+      <c r="I78" s="10">
+        <f t="shared" si="2"/>
+        <v>16157.333333333334</v>
+      </c>
+      <c r="J78" s="10">
+        <f t="shared" si="2"/>
+        <v>10887</v>
+      </c>
+    </row>
+    <row r="79" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C79" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D79" s="16"/>
-      <c r="E79" s="17">
+      <c r="D79" s="23"/>
+      <c r="E79" s="13">
         <f>(AVERAGE(E28,E53,E78))</f>
         <v>1426275.4166666667</v>
       </c>
-      <c r="F79" s="17">
+      <c r="F79" s="13">
         <f>(AVERAGE(F28,F53,F78))</f>
         <v>4806.7361111111104</v>
       </c>
-      <c r="G79" s="18">
+      <c r="G79" s="13">
         <f>(AVERAGE(G28,G53,G78))</f>
         <v>76936.222222222219</v>
       </c>
-    </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C80" s="9" t="s">
+      <c r="H79" s="13">
+        <f t="shared" ref="H79:J79" si="3">(AVERAGE(H28,H53,H78))</f>
+        <v>1756797.8888888888</v>
+      </c>
+      <c r="I79" s="13">
+        <f t="shared" si="3"/>
+        <v>5559.7361111111122</v>
+      </c>
+      <c r="J79" s="13">
+        <f t="shared" si="3"/>
+        <v>8410.6593567251457</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C80" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1">
+      <c r="D80" s="20"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14">
         <f>E79/F79</f>
         <v>296.72430183336468</v>
       </c>
-      <c r="G80" s="10"/>
-    </row>
-    <row r="81" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C81" s="11" t="s">
+      <c r="G80" s="15"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+    </row>
+    <row r="81" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D81" s="12"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13">
+      <c r="D81" s="22"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11">
         <f>E34/F34</f>
         <v>325.36025000000001</v>
       </c>
-      <c r="G81" s="14">
+      <c r="G81" s="12">
         <f>E34/G34</f>
         <v>1.0192215973567171</v>
       </c>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="H2:J2"/>
     <mergeCell ref="C80:D80"/>
     <mergeCell ref="C81:D81"/>
     <mergeCell ref="C79:D79"/>
@@ -2908,5 +3955,6 @@
     <mergeCell ref="C54:C78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
display interface simplification to allow future features
(I also begin to research new board check ideas in check_board.c)
</commit_message>
<xml_diff>
--- a/showcase assets/IQ_circuit_solver_stats.xlsx
+++ b/showcase assets/IQ_circuit_solver_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Projets_persos\Prog\C\IQ_circuit_solver\showcase assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4175B440-0A2D-4CB6-A836-20D4523FE3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C4CEFB-F5BD-4849-9920-959183642192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{22D5D88B-9009-499F-A617-719D769432EB}"/>
   </bookViews>
@@ -875,12 +875,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -888,6 +882,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -980,17 +980,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2392,7 +2392,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> is ridiculously insane, look at the total number of valid boards : V3 = 40M -&gt; V3.1 = 10M -&gt; V3.2 B = 53 000 ??? My laptop can now solve every encoded levels in less than a second, yet it's not very fast anymore.</a:t>
+            <a:t> is ridiculously insane, look at the total number of valid boards : V2 = 126M -&gt; V3 = 40M -&gt; V3.1 = 10M -&gt; V3.2 B = 53 000 ??? My laptop can now solve every encoded levels in less than a second, yet it's not very fast anymore.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3152,7 +3152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA32E1-4AE2-41F3-A97D-46388028FF7D}">
   <dimension ref="B1:L161"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
+    <sheetView topLeftCell="A135" workbookViewId="0">
       <selection activeCell="R83" sqref="R82:R83"/>
     </sheetView>
   </sheetViews>
@@ -3178,17 +3178,17 @@
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="93"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="91"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
@@ -5306,10 +5306,10 @@
       </c>
     </row>
     <row r="81" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D81" s="89" t="s">
+      <c r="D81" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="E81" s="90"/>
+      <c r="E81" s="93"/>
       <c r="F81" s="18"/>
       <c r="G81" s="18">
         <f t="shared" ref="G81:L81" si="4">SUM(G5:G28,G30:G53,G55:G78)</f>
@@ -5338,17 +5338,17 @@
     </row>
     <row r="82" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="83" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D83" s="91" t="s">
+      <c r="D83" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="E83" s="92"/>
-      <c r="F83" s="92"/>
-      <c r="G83" s="92"/>
-      <c r="H83" s="92"/>
-      <c r="I83" s="92"/>
-      <c r="J83" s="92"/>
-      <c r="K83" s="92"/>
-      <c r="L83" s="93"/>
+      <c r="E83" s="90"/>
+      <c r="F83" s="90"/>
+      <c r="G83" s="90"/>
+      <c r="H83" s="90"/>
+      <c r="I83" s="90"/>
+      <c r="J83" s="90"/>
+      <c r="K83" s="90"/>
+      <c r="L83" s="91"/>
     </row>
     <row r="84" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
@@ -7735,10 +7735,10 @@
       </c>
     </row>
     <row r="161" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D161" s="89" t="s">
+      <c r="D161" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="E161" s="90"/>
+      <c r="E161" s="93"/>
       <c r="F161" s="18" t="s">
         <v>33</v>
       </c>
@@ -7768,11 +7768,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D5:D29"/>
-    <mergeCell ref="D30:D54"/>
-    <mergeCell ref="D55:D79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D3:L3"/>
     <mergeCell ref="D135:D159"/>
     <mergeCell ref="D160:E160"/>
     <mergeCell ref="D81:E81"/>
@@ -7780,6 +7775,11 @@
     <mergeCell ref="D85:D109"/>
     <mergeCell ref="D110:D134"/>
     <mergeCell ref="D83:L83"/>
+    <mergeCell ref="D5:D29"/>
+    <mergeCell ref="D30:D54"/>
+    <mergeCell ref="D55:D79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D3:L3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -7796,8 +7796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE79279-43FE-4514-886C-88FC286043C2}">
   <dimension ref="A1:Y118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M47" workbookViewId="0">
-      <selection activeCell="AB105" sqref="AB105"/>
+    <sheetView tabSelected="1" topLeftCell="M87" workbookViewId="0">
+      <selection activeCell="AB108" sqref="AB108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13351,32 +13351,32 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="E4" s="127" t="s">
+      <c r="E4" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
     </row>
     <row r="5" spans="3:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="126" t="s">
+      <c r="E5" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126" t="s">
+      <c r="F5" s="125"/>
+      <c r="G5" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126" t="s">
+      <c r="H5" s="125"/>
+      <c r="I5" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="126"/>
+      <c r="J5" s="125"/>
     </row>
     <row r="6" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
@@ -14526,10 +14526,10 @@
       </c>
     </row>
     <row r="82" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C82" s="124" t="s">
+      <c r="C82" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="D82" s="124"/>
+      <c r="D82" s="126"/>
       <c r="E82" s="14">
         <f>AVERAGE(E7:E30,E32:E55,E57:E80)</f>
         <v>16807.150000000001</v>
@@ -14556,10 +14556,10 @@
       </c>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C83" s="125" t="s">
+      <c r="C83" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="D83" s="125"/>
+      <c r="D83" s="127"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6">
         <f>E82/F82</f>
@@ -14585,16 +14585,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C57:C81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="C7:C31"/>
     <mergeCell ref="C32:C56"/>
-    <mergeCell ref="C57:C81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
V5.0 : Added user interaction before launching the search algorithm
(it's meant to make demos of this project more enjoyable)

0) Added raylib logo introduction

1) Added graphic menu for level selection, with credits to the IQ circuit puzzle website

2) Added a playable mode when the user enters a level, with more UI (controls display)
    - free mode : user can play piece wherever he wants
    - assisted mode : each time the user plays a piece, board checks are run to see if it's a good play, and inform user about it.

3) Added UI to set up the solving algorithm before launching it.
    - FPS choice : group of toggle buttons that set the speed at which the algorithm is run (how many new valid boards per seconds), with options for unlimited FPS, and for a manual frame by frame mode.

4) FPS are still settable when the solving algorithm is running.

5) At any time, user can press the escape key to go back to level selection.
</commit_message>
<xml_diff>
--- a/showcase assets/IQ_circuit_solver_stats.xlsx
+++ b/showcase assets/IQ_circuit_solver_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Projets_persos\Prog\C\IQ_circuit_solver\showcase assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C4CEFB-F5BD-4849-9920-959183642192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3550C20A-B31E-40D6-964D-DCE2D4FA3499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{22D5D88B-9009-499F-A617-719D769432EB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22D5D88B-9009-499F-A617-719D769432EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup comments" sheetId="2" r:id="rId1"/>
@@ -875,6 +875,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -882,12 +888,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -980,17 +980,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1178,6 +1178,17 @@
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> Automated runs are done on the main display of the laptop (I later found out that it runs faster if the frames are drawn on a second display, directly linked to the GPU, rather than integrated graphics on CPU).</a:t>
+          </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -3122,7 +3133,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3132,7 +3143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC46C79C-8D6A-4FFB-B893-72DF3CB341BA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -3178,17 +3189,17 @@
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D3" s="89" t="s">
+      <c r="D3" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="91"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="93"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
@@ -5306,10 +5317,10 @@
       </c>
     </row>
     <row r="81" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D81" s="92" t="s">
+      <c r="D81" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="E81" s="93"/>
+      <c r="E81" s="90"/>
       <c r="F81" s="18"/>
       <c r="G81" s="18">
         <f t="shared" ref="G81:L81" si="4">SUM(G5:G28,G30:G53,G55:G78)</f>
@@ -5338,17 +5349,17 @@
     </row>
     <row r="82" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="83" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D83" s="89" t="s">
+      <c r="D83" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="E83" s="90"/>
-      <c r="F83" s="90"/>
-      <c r="G83" s="90"/>
-      <c r="H83" s="90"/>
-      <c r="I83" s="90"/>
-      <c r="J83" s="90"/>
-      <c r="K83" s="90"/>
-      <c r="L83" s="91"/>
+      <c r="E83" s="92"/>
+      <c r="F83" s="92"/>
+      <c r="G83" s="92"/>
+      <c r="H83" s="92"/>
+      <c r="I83" s="92"/>
+      <c r="J83" s="92"/>
+      <c r="K83" s="92"/>
+      <c r="L83" s="93"/>
     </row>
     <row r="84" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D84" s="4" t="s">
@@ -7735,10 +7746,10 @@
       </c>
     </row>
     <row r="161" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D161" s="92" t="s">
+      <c r="D161" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E161" s="93"/>
+      <c r="E161" s="90"/>
       <c r="F161" s="18" t="s">
         <v>33</v>
       </c>
@@ -7768,6 +7779,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D5:D29"/>
+    <mergeCell ref="D30:D54"/>
+    <mergeCell ref="D55:D79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D3:L3"/>
     <mergeCell ref="D135:D159"/>
     <mergeCell ref="D160:E160"/>
     <mergeCell ref="D81:E81"/>
@@ -7775,11 +7791,6 @@
     <mergeCell ref="D85:D109"/>
     <mergeCell ref="D110:D134"/>
     <mergeCell ref="D83:L83"/>
-    <mergeCell ref="D5:D29"/>
-    <mergeCell ref="D30:D54"/>
-    <mergeCell ref="D55:D79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D3:L3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -7796,7 +7807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE79279-43FE-4514-886C-88FC286043C2}">
   <dimension ref="A1:Y118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M87" workbookViewId="0">
+    <sheetView topLeftCell="M87" workbookViewId="0">
       <selection activeCell="AB108" sqref="AB108"/>
     </sheetView>
   </sheetViews>
@@ -13351,32 +13362,32 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="E4" s="124" t="s">
+      <c r="E4" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
     </row>
     <row r="5" spans="3:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="125" t="s">
+      <c r="E5" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125" t="s">
+      <c r="F5" s="126"/>
+      <c r="G5" s="126" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="125"/>
-      <c r="I5" s="125" t="s">
+      <c r="H5" s="126"/>
+      <c r="I5" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="125"/>
+      <c r="J5" s="126"/>
     </row>
     <row r="6" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
@@ -14526,10 +14537,10 @@
       </c>
     </row>
     <row r="82" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C82" s="126" t="s">
+      <c r="C82" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="D82" s="126"/>
+      <c r="D82" s="124"/>
       <c r="E82" s="14">
         <f>AVERAGE(E7:E30,E32:E55,E57:E80)</f>
         <v>16807.150000000001</v>
@@ -14556,10 +14567,10 @@
       </c>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C83" s="127" t="s">
+      <c r="C83" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="D83" s="127"/>
+      <c r="D83" s="125"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6">
         <f>E82/F82</f>
@@ -14585,16 +14596,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C7:C31"/>
+    <mergeCell ref="C32:C56"/>
     <mergeCell ref="C57:C81"/>
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="C84:D84"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C7:C31"/>
-    <mergeCell ref="C32:C56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>